<commit_message>
Update master data mahasiswa TA.xlsx
</commit_message>
<xml_diff>
--- a/master data mahasiswa TA.xlsx
+++ b/master data mahasiswa TA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbee3ff0ebd21f1/simta application/simta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="14_{530DA884-83DA-4C64-A992-12F8642618A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8510AD26-A09F-448D-97D7-58BDE6153461}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="14_{530DA884-83DA-4C64-A992-12F8642618A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B407195-77D2-4779-A00B-B322BB150690}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{9D7D56C9-3BFC-42AD-8CDB-4B7184614D5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{9D7D56C9-3BFC-42AD-8CDB-4B7184614D5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ganjil 2021-2022" sheetId="5" r:id="rId1"/>
-    <sheet name="genap 2021-2022" sheetId="6" r:id="rId2"/>
-    <sheet name="ganjil 2022-2023" sheetId="7" r:id="rId3"/>
-    <sheet name="genap 2022-2023" sheetId="10" r:id="rId4"/>
+    <sheet name="gjl 21.22" sheetId="5" r:id="rId1"/>
+    <sheet name="gnp 21.22" sheetId="6" r:id="rId2"/>
+    <sheet name="gjl 22.23" sheetId="7" r:id="rId3"/>
+    <sheet name="gnp 22.23" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -257,17 +257,9 @@
     <t>irenedyah@student.ittelkom-sby.ac.id</t>
   </si>
   <si>
-    <t>Perancangan Website Angkutan Umum Dengan Metode Prototyping Sebagai Upaya Mengurangi Interaksi Pengguna Public 
-Transportation Di Era Pandemi Covid-19 (Studi Kasus Kota Tuban Jawa Timur)</t>
-  </si>
-  <si>
     <t>Evaluasi Pengalaman Pengguna Aplikasi Mobile Xgracias Telkom Campus Menggunakan User Experience Questionnaire (UEQ)</t>
   </si>
   <si>
-    <t>Perancangan User Interface Pada Sistem Informasi Akademik Igracias Menggunakan Pendekatan User Centered Design Di 
-Institute Teknologi Telkom Surabaya</t>
-  </si>
-  <si>
     <t>andikalaksana2000@gmail.com</t>
   </si>
   <si>
@@ -323,6 +315,12 @@
   </si>
   <si>
     <t>Evaluasi Pengalaman Pengguna Aplikasi Siamo (Sistem Informasi Administrasi Manajemen Operasi) Dengan Menggunakan Metode System Usability Scale (SUS) Dan Usability Testing (Studi Kasus: PMR Dan KSR di Kota Surabaya)</t>
+  </si>
+  <si>
+    <t>Perancangan Website Angkutan Umum Dengan Metode Prototyping Sebagai Upaya Mengurangi Interaksi Pengguna Public Transportation Di Era Pandemi Covid-19 (Studi Kasus Kota Tuban Jawa Timur)</t>
+  </si>
+  <si>
+    <t>Perancangan User Interface Pada Sistem Informasi Akademik Igracias Menggunakan Pendekatan User Centered Design Di Institute Teknologi Telkom Surabaya</t>
   </si>
 </sst>
 </file>
@@ -816,16 +814,16 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -851,10 +849,10 @@
         <v>70</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>3</v>
@@ -877,10 +875,10 @@
         <v>69</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>3</v>
@@ -901,8 +899,8 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,16 +924,16 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -958,16 +956,16 @@
         <v>44593</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -981,10 +979,10 @@
         <v>44593</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>3</v>
@@ -1001,16 +999,16 @@
         <v>44593</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>1204180007</v>
       </c>
@@ -1021,13 +1019,13 @@
         <v>44593</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>3</v>
@@ -1044,10 +1042,10 @@
         <v>44593</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>3</v>
@@ -1064,10 +1062,10 @@
         <v>44593</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>3</v>
@@ -1084,16 +1082,16 @@
         <v>44593</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>1204180024</v>
       </c>
@@ -1104,13 +1102,13 @@
         <v>44593</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>3</v>
@@ -1127,10 +1125,10 @@
         <v>44593</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>3</v>
@@ -1147,10 +1145,10 @@
         <v>44593</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>3</v>
@@ -1167,16 +1165,16 @@
         <v>44593</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>1204180031</v>
       </c>
@@ -1187,13 +1185,13 @@
         <v>44593</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>86</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>3</v>
@@ -1210,10 +1208,10 @@
         <v>44593</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>3</v>
@@ -1230,10 +1228,10 @@
         <v>44593</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>3</v>
@@ -1250,16 +1248,16 @@
         <v>44593</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1273,10 +1271,10 @@
         <v>44593</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>3</v>
@@ -1293,10 +1291,10 @@
         <v>44593</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>3</v>
@@ -1313,10 +1311,10 @@
         <v>44593</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>3</v>
@@ -1330,10 +1328,10 @@
         <v>23</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1344,10 +1342,10 @@
         <v>24</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1358,10 +1356,10 @@
         <v>25</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1372,10 +1370,10 @@
         <v>26</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1386,10 +1384,10 @@
         <v>27</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1400,10 +1398,10 @@
         <v>28</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1416,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C966F923-3B2B-4299-B621-1C0A34313445}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1441,16 +1439,16 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -1473,13 +1471,13 @@
         <v>44743</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4"/>
     </row>
@@ -1494,13 +1492,13 @@
         <v>44743</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -1515,13 +1513,13 @@
         <v>44743</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -1537,10 +1535,10 @@
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1556,10 +1554,10 @@
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -1575,10 +1573,10 @@
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -1594,10 +1592,10 @@
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -1613,10 +1611,10 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1632,10 +1630,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1651,10 +1649,10 @@
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -1670,10 +1668,10 @@
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -1689,10 +1687,10 @@
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -1708,10 +1706,10 @@
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1727,10 +1725,10 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -1746,10 +1744,10 @@
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1765,10 +1763,10 @@
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1784,10 +1782,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1803,10 +1801,10 @@
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1822,10 +1820,10 @@
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1841,10 +1839,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -1860,10 +1858,10 @@
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -1879,10 +1877,10 @@
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -1898,10 +1896,10 @@
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -1917,10 +1915,10 @@
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G25" s="4"/>
     </row>
@@ -1936,10 +1934,10 @@
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -1955,10 +1953,10 @@
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1974,10 +1972,10 @@
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -1993,10 +1991,10 @@
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" s="4"/>
     </row>
@@ -2012,10 +2010,10 @@
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -2031,10 +2029,10 @@
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -2050,10 +2048,10 @@
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -2069,10 +2067,10 @@
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -2088,10 +2086,10 @@
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -2107,10 +2105,10 @@
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G35" s="4"/>
     </row>
@@ -2126,10 +2124,10 @@
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G36" s="4"/>
     </row>
@@ -2145,10 +2143,10 @@
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G37" s="4"/>
     </row>
@@ -2165,9 +2163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CC19EE-8F0D-4BC1-80CB-7F34D94B7007}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2190,16 +2188,16 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>

</xml_diff>